<commit_message>
cập nhật File kế hoạch
</commit_message>
<xml_diff>
--- a/KeHoachThucHien.xlsx
+++ b/KeHoachThucHien.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TLCN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TLCN\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250E8598-3F62-4036-B53F-2F47DB743342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CD2EBF-67CC-4B94-A430-B008FB913189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="116">
   <si>
     <t>STT</t>
   </si>
@@ -456,19 +456,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -477,19 +477,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,9 +1364,7 @@
       <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1388,9 +1386,7 @@
       <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
         <v>34</v>
       </c>
@@ -1410,9 +1406,7 @@
       <c r="C19" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
         <v>34</v>
       </c>
@@ -1432,9 +1426,7 @@
       <c r="C20" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1454,9 +1446,7 @@
       <c r="C21" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
         <v>34</v>
       </c>
@@ -1476,9 +1466,7 @@
       <c r="C22" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
         <v>34</v>
       </c>
@@ -1498,9 +1486,7 @@
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
         <v>34</v>
       </c>
@@ -1520,9 +1506,7 @@
       <c r="C24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
         <v>34</v>
       </c>
@@ -1542,9 +1526,7 @@
       <c r="C25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="D25" s="12"/>
       <c r="E25" s="12" t="s">
         <v>34</v>
       </c>
@@ -1571,9 +1553,7 @@
       <c r="D26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="15" t="s">
         <v>61</v>
       </c>
@@ -1595,9 +1575,7 @@
       <c r="D27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="15" t="s">
         <v>61</v>
       </c>
@@ -1617,9 +1595,7 @@
       <c r="D28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="15" t="s">
         <v>93</v>
       </c>
@@ -1639,9 +1615,7 @@
       <c r="D29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="15" t="s">
         <v>93</v>
       </c>
@@ -1661,9 +1635,7 @@
       <c r="D30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E30" s="5"/>
       <c r="F30" s="15" t="s">
         <v>93</v>
       </c>
@@ -1683,9 +1655,7 @@
       <c r="D31" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E31" s="5"/>
       <c r="F31" s="15" t="s">
         <v>95</v>
       </c>
@@ -1705,9 +1675,7 @@
       <c r="D32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="15" t="s">
         <v>95</v>
       </c>
@@ -1727,9 +1695,7 @@
       <c r="D33" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="15" t="s">
         <v>96</v>
       </c>
@@ -1749,9 +1715,7 @@
       <c r="D34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E34" s="5"/>
       <c r="F34" s="15" t="s">
         <v>98</v>
       </c>
@@ -1771,9 +1735,7 @@
       <c r="D35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="9" t="s">
         <v>99</v>
       </c>
@@ -1793,9 +1755,7 @@
       <c r="D36" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E36" s="5"/>
       <c r="F36" s="9" t="s">
         <v>99</v>
       </c>
@@ -1815,9 +1775,7 @@
       <c r="D37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="9" t="s">
         <v>100</v>
       </c>
@@ -1837,9 +1795,7 @@
       <c r="D38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="E38" s="5"/>
       <c r="F38" s="9" t="s">
         <v>100</v>
       </c>
@@ -1859,9 +1815,7 @@
       <c r="D39" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="E39" s="12"/>
       <c r="F39" s="14" t="s">
         <v>101</v>
       </c>

</xml_diff>